<commit_message>
feat (excel): store to db
Stored all the users on the list into the database and send them a
communication email to welcome them to the company.

 #22 from #16
</commit_message>
<xml_diff>
--- a/uploads/Boo21.xlsx
+++ b/uploads/Boo21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janvi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5979D58-1C3D-4EB5-AF6B-3E838A9CA10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF87593-B50F-4D9C-8D05-90267095FBDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
-    <t>Dulce</t>
-  </si>
-  <si>
     <t>Mara</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Fallon</t>
   </si>
   <si>
-    <t>abril@gmail.com</t>
-  </si>
-  <si>
     <t>hashimoto@abc.com</t>
   </si>
   <si>
@@ -143,6 +137,12 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>Rouge</t>
+  </si>
+  <si>
+    <t>janvierntwali@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -517,15 +517,15 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.5703125"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
     <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
@@ -534,25 +534,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -560,25 +560,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>250724955240</v>
       </c>
       <c r="E2">
-        <v>1199880088550020</v>
+        <v>1188773399330050</v>
       </c>
       <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -586,25 +586,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>250724955240</v>
+        <v>250724955242</v>
       </c>
       <c r="E3">
-        <v>1199880088550020</v>
+        <v>1188337740373500</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -612,25 +612,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>250724955240</v>
+        <v>250724955241</v>
       </c>
       <c r="E4">
-        <v>1199880088550020</v>
+        <v>1277422464446730</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,25 +638,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>250724955240</v>
+        <v>250724955243</v>
       </c>
       <c r="E5">
-        <v>1199880088550020</v>
+        <v>1199800819494020</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -664,25 +664,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>250724955240</v>
+        <v>250724955244</v>
       </c>
       <c r="E6">
-        <v>1199880088550020</v>
+        <v>1947300889050020</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -690,25 +690,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>250724955240</v>
+        <v>250724955246</v>
       </c>
       <c r="E7">
-        <v>1199880088550020</v>
+        <v>1483957385758350</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -716,25 +716,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>250724955240</v>
+        <v>250724955245</v>
       </c>
       <c r="E8">
-        <v>1199880088550020</v>
+        <v>1947736457285720</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -742,25 +742,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>250724955240</v>
+        <v>250724955247</v>
       </c>
       <c r="E9">
-        <v>1199880088550020</v>
+        <v>1893857385003840</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -768,25 +768,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>250724955240</v>
+        <v>250724955248</v>
       </c>
       <c r="E10">
-        <v>1199880088550020</v>
+        <v>7383748728278500</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -794,25 +794,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>250724955240</v>
+        <v>250724955249</v>
       </c>
       <c r="E11">
-        <v>1199880088550020</v>
+        <v>1199880081551020</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
     <hyperlink ref="C11" r:id="rId10" xr:uid="{3B4C6783-F76C-4012-8158-36A79B43D07A}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>